<commit_message>
Done for now --- merge- and quicksort do not work yet.
</commit_message>
<xml_diff>
--- a/Lab7-Timings.xlsx
+++ b/Lab7-Timings.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2030\2030-GA-Files\2030-GA-Files\lab\instructs-NEW\lab7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwill\Documents\GitHub\Lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{533B807F-7BB1-49BF-BC6B-75E9709D5697}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9345" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8320" windowHeight="1670" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -413,25 +414,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.58203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -442,7 +443,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -451,7 +452,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -474,23 +475,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>5300000</v>
       </c>
       <c r="C5">
         <f>2*B5</f>
-        <v>0</v>
+        <v>10600000</v>
       </c>
       <c r="E5">
         <f>2*C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21200000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -503,46 +504,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="B7">
+        <v>15000</v>
+      </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>18100</v>
+      </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>36200</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>72400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>21500</v>
+      </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43000</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>86000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Some comments in the code
</commit_message>
<xml_diff>
--- a/Lab7-Timings.xlsx
+++ b/Lab7-Timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwill\Documents\GitHub\Lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{533B807F-7BB1-49BF-BC6B-75E9709D5697}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E55C730F-D883-4BCE-9D19-C16B423EB341}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8320" windowHeight="1670" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>